<commit_message>
Added further tools and plots
EstuaryDB - Changed Case tab to Data and Models tabs. added load for spatial data.
EDBimport - flat tables now use muitTableImport and this class handles vector data with each estuary being a separate case.
Added format function files for zm data and images. reworked edb_regression_analysis and edb_regression_plot for revised data format.
edb_user_tools - get_Table now calls table_figure in dstable. implemented convergence analysis.
edb_user_plots - scatter, type and range plots made external functions along with checkdimensions. Added range plot
</commit_message>
<xml_diff>
--- a/app/example/Estuary_DSproperties.xlsx
+++ b/app/example/Estuary_DSproperties.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fef2681617fd0817/Work/Research/Estuary/Form/Equilibrium/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Matlab Code\muiModels\EstuaryDB\app\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="129" documentId="13_ncr:1_{BC9EA38A-1ED8-4B01-848F-7AF58F9683C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1E43120-E580-4408-911E-DB8F68CD9443}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A27EEF0-E7B6-472B-9302-03C77E50DAFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5590" yWindow="3420" windowWidth="28800" windowHeight="15370" xr2:uid="{0BAB9EBC-37C2-4AE1-9E72-4C5423A704D3}"/>
+    <workbookView xWindow="5760" yWindow="3250" windowWidth="28800" windowHeight="15370" activeTab="1" xr2:uid="{0BAB9EBC-37C2-4AE1-9E72-4C5423A704D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Class" sheetId="1" r:id="rId1"/>
@@ -707,8 +707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8224E8D-F3E1-4142-B50F-34380C1C9DAB}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -823,67 +823,40 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="12"/>
+      <c r="C7"/>
+      <c r="E7"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="11"/>
+      <c r="C8"/>
+      <c r="E8"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="12"/>
+      <c r="C9"/>
+      <c r="E9"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="11"/>
+      <c r="C10"/>
+      <c r="E10"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="12"/>
+      <c r="C11"/>
+      <c r="E11"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="11"/>
+      <c r="C12"/>
+      <c r="E12"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="1"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="12"/>
+      <c r="C13"/>
+      <c r="E13"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="11"/>
+      <c r="C14"/>
+      <c r="E14"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="12"/>
+      <c r="C15"/>
+      <c r="E15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -894,9 +867,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9365A27-D618-4F3B-B9D4-62C6ED011B71}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>